<commit_message>
Updated bom, slightchanges to footprint indicators
</commit_message>
<xml_diff>
--- a/V2.1/BOM/Pierogi Nixie-6 BOM.xlsx
+++ b/V2.1/BOM/Pierogi Nixie-6 BOM.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="86">
+  <si>
+    <t>Part ID</t>
+  </si>
   <si>
     <t>Part Description</t>
   </si>
@@ -85,10 +88,10 @@
     <t>IC9</t>
   </si>
   <si>
-    <t>L7805CD2T-TR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/L7805CD2T-TR/585695?s=N4IgTCBcDaIDIHYAcAGArAYQCJgCoFpcAlEAXQF8g</t>
+    <t>TPS54302DDCT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/TPS54302DDCT/6123254</t>
   </si>
   <si>
     <t>N1, N2, N3, N4, N5, N6</t>
@@ -118,22 +121,49 @@
     <t>https://www.digikey.com/en/products/detail/c-k/pts-647-sn50-smtr2-lfs/9649857</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C11</t>
+    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C11, C13, C14</t>
   </si>
   <si>
     <t>0805 100nf/.1uF Capacitor</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/C0805C104M3RAC7800/2211748</t>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
   </si>
   <si>
     <t>C10</t>
   </si>
   <si>
-    <t>0805 .33uF Capacitor</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21B334KBFNNNE/3886781</t>
+    <t>47uF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kyocera-avx/F931A476KAA/4005057</t>
+  </si>
+  <si>
+    <t>C11, C12</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21A106KOQNNNE/3886754</t>
+  </si>
+  <si>
+    <t>C15, C16</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21A226KOQNNNE/5961010</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>75pF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/CC0805JRNPO9BN750/5884054</t>
   </si>
   <si>
     <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11</t>
@@ -142,7 +172,61 @@
     <t>0805 10K Resistor</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/yageo/RC0805JR-0710KL/728241</t>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/RCS080510K0FKEA/5866991</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>511K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RK73H2ARTTD5113F/12548650</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>105K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RK73H2ATTD1053F/10234720</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>49.9 ohm</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/CRCW080549R9FKEAHP/2222324</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/SG73P2ATTD1003F/10188411</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>13.3K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/CRCW080513K3FKEAHP/2227086</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/abracon-llc/ASPI-0630LR-100M-T15/3059602</t>
   </si>
   <si>
     <t>Misc</t>
@@ -154,12 +238,6 @@
     <t>https://www.digikey.com/en/products/detail/on-shore-technology-inc/ED16DT/4147596</t>
   </si>
   <si>
-    <t>Panel Mount Switch</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/bulgin/C1300ABBB-602AW/5057976</t>
-  </si>
-  <si>
     <t>20 pin male header</t>
   </si>
   <si>
@@ -191,9 +269,6 @@
   </si>
   <si>
     <t>Final Total:</t>
-  </si>
-  <si>
-    <t>DOES NOT INCLUDE SHIPPING AND TAX</t>
   </si>
 </sst>
 </file>
@@ -250,8 +325,13 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
@@ -260,13 +340,13 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -501,37 +581,39 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="36.38"/>
+    <col customWidth="1" min="1" max="1" width="39.88"/>
     <col customWidth="1" min="2" max="2" width="22.38"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6">
         <v>4.0</v>
@@ -540,19 +622,19 @@
         <v>1.0</v>
       </c>
       <c r="F2" s="7">
-        <f t="shared" ref="F2:F21" si="1">D2*E2</f>
+        <f t="shared" ref="F2:F29" si="1">D2*E2</f>
         <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="6">
         <v>0.21</v>
@@ -567,13 +649,13 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6">
         <v>0.92</v>
@@ -588,13 +670,13 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6">
         <v>2.98</v>
@@ -609,13 +691,13 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="6">
         <v>1.62</v>
@@ -630,13 +712,13 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="6">
         <v>9.81</v>
@@ -651,34 +733,34 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="6">
-        <v>1.02</v>
+        <v>2.01</v>
       </c>
       <c r="E8" s="4">
         <v>1.0</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="1"/>
-        <v>1.02</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="6">
         <v>10.0</v>
@@ -693,13 +775,13 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="6">
         <v>1.34</v>
@@ -714,13 +796,13 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D11" s="6">
         <v>0.2</v>
@@ -735,226 +817,389 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="8" t="s">
         <v>37</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="D12" s="6">
         <v>0.1</v>
       </c>
       <c r="E12" s="4">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" s="6">
-        <v>0.1</v>
+        <v>0.72</v>
       </c>
       <c r="E13" s="4">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14" s="6">
         <v>0.1</v>
       </c>
       <c r="E14" s="4">
-        <v>11.0</v>
+        <v>2.0</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="1"/>
-        <v>1.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" s="6">
-        <v>0.26</v>
+        <v>0.33</v>
       </c>
       <c r="E15" s="4">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="1"/>
-        <v>1.56</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16" s="6">
-        <v>2.77</v>
+        <v>0.14</v>
       </c>
       <c r="E16" s="4">
         <v>1.0</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="1"/>
-        <v>2.77</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="D17" s="6">
-        <v>0.32</v>
+        <v>0.1</v>
       </c>
       <c r="E17" s="4">
-        <v>6.0</v>
+        <v>11.0</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="1"/>
-        <v>1.92</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D18" s="6">
-        <v>1.23</v>
+        <v>0.19</v>
       </c>
       <c r="E18" s="4">
         <v>1.0</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
-        <v>1.23</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D19" s="6">
-        <v>0.37</v>
+        <v>0.1</v>
       </c>
       <c r="E19" s="4">
         <v>1.0</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="1"/>
-        <v>0.37</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D20" s="6">
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
       <c r="E20" s="4">
         <v>1.0</v>
       </c>
       <c r="F20" s="7">
         <f t="shared" si="1"/>
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>28</v>
+        <v>64</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="D21" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F22" s="7">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F23" s="7">
+        <f t="shared" si="1"/>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.26</v>
+      </c>
+      <c r="E24" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F24" s="7">
+        <f t="shared" si="1"/>
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="E25" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F25" s="7">
+        <f t="shared" si="1"/>
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1.23</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F26" s="7">
+        <f t="shared" si="1"/>
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.37</v>
+      </c>
+      <c r="E27" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F27" s="7">
+        <f t="shared" si="1"/>
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F28" s="7">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="6">
         <v>7.0</v>
       </c>
-      <c r="E21" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F21" s="7">
+      <c r="E29" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F29" s="7">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="22">
-      <c r="E22" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="7">
-        <f>Sum(F2:F21)</f>
-        <v>116.06</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="E23" s="4" t="s">
-        <v>60</v>
+    <row r="30">
+      <c r="E30" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="7">
+        <f>Sum(F2:F29)</f>
+        <v>124.07</v>
       </c>
     </row>
   </sheetData>
@@ -977,7 +1222,15 @@
     <hyperlink r:id="rId16" ref="C18"/>
     <hyperlink r:id="rId17" ref="C19"/>
     <hyperlink r:id="rId18" ref="C20"/>
+    <hyperlink r:id="rId19" ref="C21"/>
+    <hyperlink r:id="rId20" ref="C22"/>
+    <hyperlink r:id="rId21" ref="C23"/>
+    <hyperlink r:id="rId22" ref="C24"/>
+    <hyperlink r:id="rId23" ref="C25"/>
+    <hyperlink r:id="rId24" ref="C26"/>
+    <hyperlink r:id="rId25" ref="C27"/>
+    <hyperlink r:id="rId26" ref="C28"/>
   </hyperlinks>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>